<commit_message>
cleaning the city survey data
</commit_message>
<xml_diff>
--- a/final_project/1996-2017_City_Survey_Codebook_DataDictionary.xlsx
+++ b/final_project/1996-2017_City_Survey_Codebook_DataDictionary.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11015"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\City Performance\CP Projects\Citywide Projects\City Survey\_2017 Survey\10. From CC&amp;G\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizchan/ds_foundations/final_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC7F1D74-1ADA-104A-8583-A87B845D57FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-312" yWindow="60" windowWidth="16152" windowHeight="10236"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Codebook" sheetId="2" r:id="rId1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Kyle Patterson</author>
   </authors>
   <commentList>
-    <comment ref="A25" authorId="0" shapeId="0">
+    <comment ref="A25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1067,9 +1068,6 @@
   </si>
   <si>
     <t>Do you have any (long term) physical conditions that limit your activities</t>
-  </si>
-  <si>
-    <t>diablement</t>
   </si>
   <si>
     <t>mentally disabled</t>
@@ -2542,11 +2540,14 @@
 Survey methodology was changed in 2015 from a mail to a phone survey. Comparisons to previous years should be interpreted with caution. Results should be weighted using the variable finweigh in order to adjust for demographic differences between the City Survey sample and San Francisco's population. Please note that survey results were originally reported as unweighted until 2000. From 2000 onward, all City Survey results were reweighted with the exception of data from 1996 and 2011. For ease of use, finweigh has been coded with a value of one for these years. Detailed information on weighting can be found in Survey Process and Methodology section of the 2017 City Survey. 
 For more information regarding San Francisco City Survey 1996-2017 Database, please visit the City Survey website at  http://www.sfgov.org/citysurvey or contact the San Francisco Controller's Office at 415-554-7463 or citysurvey@sfgov.org.</t>
   </si>
+  <si>
+    <t>disablement</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -3532,29 +3533,29 @@
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent1 2" xfId="47"/>
+    <cellStyle name="20% - Accent1 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="20% - Accent2" xfId="24" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2 2" xfId="49"/>
+    <cellStyle name="20% - Accent2 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="20% - Accent3" xfId="28" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3 2" xfId="51"/>
+    <cellStyle name="20% - Accent3 2" xfId="51" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
     <cellStyle name="20% - Accent4" xfId="32" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4 2" xfId="53"/>
+    <cellStyle name="20% - Accent4 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="20% - Accent5" xfId="36" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5 2" xfId="55"/>
+    <cellStyle name="20% - Accent5 2" xfId="55" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="20% - Accent6" xfId="40" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6 2" xfId="57"/>
+    <cellStyle name="20% - Accent6 2" xfId="57" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
     <cellStyle name="40% - Accent1" xfId="21" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1 2" xfId="48"/>
+    <cellStyle name="40% - Accent1 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="40% - Accent2" xfId="25" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2 2" xfId="50"/>
+    <cellStyle name="40% - Accent2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
     <cellStyle name="40% - Accent3" xfId="29" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3 2" xfId="52"/>
+    <cellStyle name="40% - Accent3 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="40% - Accent4" xfId="33" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4 2" xfId="54"/>
+    <cellStyle name="40% - Accent4 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
     <cellStyle name="40% - Accent5" xfId="37" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5 2" xfId="56"/>
+    <cellStyle name="40% - Accent5 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
     <cellStyle name="40% - Accent6" xfId="41" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6 2" xfId="58"/>
+    <cellStyle name="40% - Accent6 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
     <cellStyle name="60% - Accent1" xfId="22" builtinId="32" customBuiltin="1"/>
     <cellStyle name="60% - Accent2" xfId="26" builtinId="36" customBuiltin="1"/>
     <cellStyle name="60% - Accent3" xfId="30" builtinId="40" customBuiltin="1"/>
@@ -3580,15 +3581,15 @@
     <cellStyle name="Linked Cell" xfId="14" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="10" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal 3" xfId="1"/>
-    <cellStyle name="Normal 4" xfId="43"/>
-    <cellStyle name="Normal 4 2" xfId="60"/>
-    <cellStyle name="Normal 5" xfId="59"/>
-    <cellStyle name="Normal 6" xfId="45"/>
-    <cellStyle name="Note 2" xfId="44"/>
-    <cellStyle name="Note 2 2" xfId="61"/>
-    <cellStyle name="Note 3" xfId="46"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="Normal 4" xfId="43" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="Normal 4 2" xfId="60" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="Normal 5" xfId="59" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 6" xfId="45" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="Note 2" xfId="44" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="Note 2 2" xfId="61" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="Note 3" xfId="46" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
     <cellStyle name="Output" xfId="12" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="3" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="18" builtinId="25" customBuiltin="1"/>
@@ -3932,35 +3933,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:V99"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <pane ySplit="4" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K113" sqref="K113"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="11" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.6640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="7" style="24" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="25.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="7.109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.44140625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.83203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="2" customWidth="1"/>
     <col min="9" max="9" width="8" style="2" customWidth="1"/>
     <col min="10" max="10" width="39.6640625" style="2" customWidth="1"/>
     <col min="11" max="11" width="10" style="1" customWidth="1"/>
     <col min="12" max="12" width="45.6640625" style="1" customWidth="1"/>
-    <col min="13" max="22" width="8.88671875" style="1"/>
-    <col min="23" max="16384" width="8.88671875" style="2"/>
+    <col min="13" max="22" width="8.83203125" style="1"/>
+    <col min="23" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="73" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B1" s="74"/>
       <c r="C1" s="74"/>
@@ -3974,9 +3976,9 @@
       <c r="K1" s="3"/>
       <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:22" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="108.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="76" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B2" s="76"/>
       <c r="C2" s="76"/>
@@ -3990,7 +3992,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="4"/>
     </row>
-    <row r="3" spans="1:22" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A3" s="77"/>
       <c r="B3" s="77"/>
       <c r="C3" s="77"/>
@@ -4004,7 +4006,7 @@
       <c r="K3" s="7"/>
       <c r="L3" s="8"/>
     </row>
-    <row r="4" spans="1:22" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
         <v>68</v>
       </c>
@@ -4042,7 +4044,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="35" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A5" s="33" t="s">
         <v>0</v>
       </c>
@@ -4070,7 +4072,7 @@
       <c r="I5" s="13"/>
       <c r="J5" s="11"/>
       <c r="K5" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L5" s="34"/>
       <c r="M5" s="19"/>
@@ -4084,7 +4086,7 @@
       <c r="U5" s="19"/>
       <c r="V5" s="19"/>
     </row>
-    <row r="6" spans="1:22" s="35" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="35" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
       <c r="A6" s="33" t="s">
         <v>1</v>
       </c>
@@ -4112,7 +4114,7 @@
       <c r="I6" s="13"/>
       <c r="J6" s="11"/>
       <c r="K6" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L6" s="34"/>
       <c r="M6" s="19"/>
@@ -4126,7 +4128,7 @@
       <c r="U6" s="19"/>
       <c r="V6" s="19"/>
     </row>
-    <row r="7" spans="1:22" s="35" customFormat="1" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="35" customFormat="1" ht="65.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="33" t="s">
         <v>2</v>
       </c>
@@ -4158,10 +4160,10 @@
         <v>88</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L7" s="34" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
@@ -4174,7 +4176,7 @@
       <c r="U7" s="19"/>
       <c r="V7" s="19"/>
     </row>
-    <row r="8" spans="1:22" s="35" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="35" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A8" s="33" t="s">
         <v>3</v>
       </c>
@@ -4203,10 +4205,10 @@
         <v>87</v>
       </c>
       <c r="J8" s="11" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K8" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="L8" s="34" t="s">
         <v>222</v>
@@ -4222,7 +4224,7 @@
       <c r="U8" s="19"/>
       <c r="V8" s="19"/>
     </row>
-    <row r="9" spans="1:22" s="35" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="35" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A9" s="33" t="s">
         <v>4</v>
       </c>
@@ -4250,7 +4252,7 @@
       <c r="I9" s="13"/>
       <c r="J9" s="11"/>
       <c r="K9" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L9" s="34" t="s">
         <v>92</v>
@@ -4266,7 +4268,7 @@
       <c r="U9" s="19"/>
       <c r="V9" s="19"/>
     </row>
-    <row r="10" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A10" s="33" t="s">
         <v>5</v>
       </c>
@@ -4295,7 +4297,7 @@
         <v>96</v>
       </c>
       <c r="J10" s="11" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K10" s="14" t="s">
         <v>221</v>
@@ -4314,7 +4316,7 @@
       <c r="U10" s="19"/>
       <c r="V10" s="19"/>
     </row>
-    <row r="11" spans="1:22" s="35" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" s="35" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A11" s="36" t="s">
         <v>58</v>
       </c>
@@ -4343,7 +4345,7 @@
         <v>112</v>
       </c>
       <c r="J11" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K11" s="45" t="s">
         <v>244</v>
@@ -4360,9 +4362,9 @@
       <c r="U11" s="19"/>
       <c r="V11" s="19"/>
     </row>
-    <row r="12" spans="1:22" s="35" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="35" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A12" s="36" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>93</v>
@@ -4371,10 +4373,10 @@
         <v>11</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>85</v>
@@ -4389,13 +4391,13 @@
         <v>112</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K12" s="45">
         <v>2017</v>
       </c>
       <c r="L12" s="45" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M12" s="19"/>
       <c r="N12" s="19"/>
@@ -4408,9 +4410,9 @@
       <c r="U12" s="19"/>
       <c r="V12" s="19"/>
     </row>
-    <row r="13" spans="1:22" s="35" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="35" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A13" s="36" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>93</v>
@@ -4419,10 +4421,10 @@
         <v>12</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>85</v>
@@ -4437,13 +4439,13 @@
         <v>112</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K13" s="45">
         <v>2017</v>
       </c>
       <c r="L13" s="45" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="M13" s="19"/>
       <c r="N13" s="19"/>
@@ -4456,9 +4458,9 @@
       <c r="U13" s="19"/>
       <c r="V13" s="19"/>
     </row>
-    <row r="14" spans="1:22" s="35" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="35" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A14" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>93</v>
@@ -4485,10 +4487,10 @@
         <v>112</v>
       </c>
       <c r="J14" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K14" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L14" s="19"/>
       <c r="M14" s="19"/>
@@ -4502,7 +4504,7 @@
       <c r="U14" s="19"/>
       <c r="V14" s="19"/>
     </row>
-    <row r="15" spans="1:22" s="35" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" s="35" customFormat="1" ht="196" hidden="1" x14ac:dyDescent="0.15">
       <c r="A15" s="33" t="s">
         <v>6</v>
       </c>
@@ -4537,7 +4539,7 @@
         <v>224</v>
       </c>
       <c r="L15" s="34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M15" s="19"/>
       <c r="N15" s="19"/>
@@ -4550,9 +4552,9 @@
       <c r="U15" s="19"/>
       <c r="V15" s="19"/>
     </row>
-    <row r="16" spans="1:22" s="35" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="35" customFormat="1" ht="111.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="33" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>93</v>
@@ -4561,10 +4563,10 @@
         <v>15</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F16" s="34" t="s">
         <v>85</v>
@@ -4579,7 +4581,7 @@
         <v>112</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K16" s="14">
         <v>2017</v>
@@ -4596,7 +4598,7 @@
       <c r="U16" s="19"/>
       <c r="V16" s="19"/>
     </row>
-    <row r="17" spans="1:22" s="35" customFormat="1" ht="234.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" s="35" customFormat="1" ht="224" hidden="1" x14ac:dyDescent="0.15">
       <c r="A17" s="33" t="s">
         <v>7</v>
       </c>
@@ -4610,7 +4612,7 @@
         <v>100</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>85</v>
@@ -4628,10 +4630,10 @@
         <v>97</v>
       </c>
       <c r="K17" s="14" t="s">
+        <v>324</v>
+      </c>
+      <c r="L17" s="34" t="s">
         <v>325</v>
-      </c>
-      <c r="L17" s="34" t="s">
-        <v>326</v>
       </c>
       <c r="M17" s="19"/>
       <c r="N17" s="19"/>
@@ -4644,7 +4646,7 @@
       <c r="U17" s="19"/>
       <c r="V17" s="19"/>
     </row>
-    <row r="18" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A18" s="36" t="s">
         <v>8</v>
       </c>
@@ -4676,10 +4678,10 @@
         <v>103</v>
       </c>
       <c r="K18" s="14" t="s">
+        <v>315</v>
+      </c>
+      <c r="L18" s="34" t="s">
         <v>316</v>
-      </c>
-      <c r="L18" s="34" t="s">
-        <v>317</v>
       </c>
       <c r="M18" s="19"/>
       <c r="N18" s="19"/>
@@ -4692,7 +4694,7 @@
       <c r="U18" s="19"/>
       <c r="V18" s="19"/>
     </row>
-    <row r="19" spans="1:22" s="35" customFormat="1" ht="179.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" s="35" customFormat="1" ht="168" hidden="1" x14ac:dyDescent="0.15">
       <c r="A19" s="33" t="s">
         <v>9</v>
       </c>
@@ -4727,7 +4729,7 @@
         <v>220</v>
       </c>
       <c r="L19" s="34" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="M19" s="19"/>
       <c r="N19" s="19"/>
@@ -4740,7 +4742,7 @@
       <c r="U19" s="19"/>
       <c r="V19" s="19"/>
     </row>
-    <row r="20" spans="1:22" s="35" customFormat="1" ht="262.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" s="35" customFormat="1" ht="224" hidden="1" x14ac:dyDescent="0.15">
       <c r="A20" s="33" t="s">
         <v>10</v>
       </c>
@@ -4772,10 +4774,10 @@
         <v>97</v>
       </c>
       <c r="K20" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L20" s="34" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="M20" s="19"/>
       <c r="N20" s="19"/>
@@ -4788,7 +4790,7 @@
       <c r="U20" s="19"/>
       <c r="V20" s="19"/>
     </row>
-    <row r="21" spans="1:22" s="35" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" s="35" customFormat="1" ht="133.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="33" t="s">
         <v>11</v>
       </c>
@@ -4817,13 +4819,13 @@
         <v>112</v>
       </c>
       <c r="J21" s="11" t="s">
+        <v>329</v>
+      </c>
+      <c r="K21" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="K21" s="14" t="s">
+      <c r="L21" s="34" t="s">
         <v>331</v>
-      </c>
-      <c r="L21" s="34" t="s">
-        <v>332</v>
       </c>
       <c r="M21" s="19"/>
       <c r="N21" s="19"/>
@@ -4836,7 +4838,7 @@
       <c r="U21" s="19"/>
       <c r="V21" s="19"/>
     </row>
-    <row r="22" spans="1:22" s="35" customFormat="1" ht="303.60000000000002" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" s="35" customFormat="1" ht="293" hidden="1" x14ac:dyDescent="0.15">
       <c r="A22" s="33" t="s">
         <v>12</v>
       </c>
@@ -4868,10 +4870,10 @@
         <v>117</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L22" s="34" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="M22" s="19"/>
       <c r="N22" s="19"/>
@@ -4884,7 +4886,7 @@
       <c r="U22" s="19"/>
       <c r="V22" s="19"/>
     </row>
-    <row r="23" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A23" s="36" t="s">
         <v>13</v>
       </c>
@@ -4898,7 +4900,7 @@
         <v>118</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>85</v>
@@ -4916,10 +4918,10 @@
         <v>103</v>
       </c>
       <c r="K23" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L23" s="34" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M23" s="19"/>
       <c r="N23" s="19"/>
@@ -4932,7 +4934,7 @@
       <c r="U23" s="19"/>
       <c r="V23" s="19"/>
     </row>
-    <row r="24" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A24" s="36" t="s">
         <v>14</v>
       </c>
@@ -4964,10 +4966,10 @@
         <v>103</v>
       </c>
       <c r="K24" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L24" s="34" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M24" s="19"/>
       <c r="N24" s="19"/>
@@ -4980,7 +4982,7 @@
       <c r="U24" s="19"/>
       <c r="V24" s="19"/>
     </row>
-    <row r="25" spans="1:22" s="19" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" s="19" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A25" s="36" t="s">
         <v>15</v>
       </c>
@@ -4994,7 +4996,7 @@
         <v>121</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F25" s="34" t="s">
         <v>85</v>
@@ -5012,15 +5014,15 @@
         <v>103</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L25" s="34" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" s="19" customFormat="1" ht="81" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="36" t="s">
         <v>340</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" s="19" customFormat="1" ht="81" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="36" t="s">
-        <v>341</v>
       </c>
       <c r="B26" s="41" t="s">
         <v>105</v>
@@ -5029,10 +5031,10 @@
         <v>23</v>
       </c>
       <c r="D26" s="41" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F26" s="11" t="s">
         <v>85</v>
@@ -5047,16 +5049,16 @@
         <v>112</v>
       </c>
       <c r="J26" s="34" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K26" s="14">
         <v>2017</v>
       </c>
       <c r="L26" s="34"/>
     </row>
-    <row r="27" spans="1:22" s="19" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" s="19" customFormat="1" ht="82.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="36" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B27" s="41" t="s">
         <v>105</v>
@@ -5065,10 +5067,10 @@
         <v>24</v>
       </c>
       <c r="D27" s="41" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>85</v>
@@ -5083,14 +5085,14 @@
         <v>112</v>
       </c>
       <c r="J27" s="34" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="K27" s="14">
         <v>2017</v>
       </c>
       <c r="L27" s="34"/>
     </row>
-    <row r="28" spans="1:22" s="35" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" s="35" customFormat="1" ht="123" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="33" t="s">
         <v>16</v>
       </c>
@@ -5122,10 +5124,10 @@
         <v>97</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L28" s="34" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -5138,7 +5140,7 @@
       <c r="U28" s="19"/>
       <c r="V28" s="19"/>
     </row>
-    <row r="29" spans="1:22" s="35" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" s="35" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.15">
       <c r="A29" s="33" t="s">
         <v>17</v>
       </c>
@@ -5170,10 +5172,10 @@
         <v>97</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L29" s="34" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="M29" s="19"/>
       <c r="N29" s="19"/>
@@ -5186,7 +5188,7 @@
       <c r="U29" s="19"/>
       <c r="V29" s="19"/>
     </row>
-    <row r="30" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A30" s="33" t="s">
         <v>18</v>
       </c>
@@ -5218,10 +5220,10 @@
         <v>129</v>
       </c>
       <c r="K30" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L30" s="34" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M30" s="19"/>
       <c r="N30" s="19"/>
@@ -5234,7 +5236,7 @@
       <c r="U30" s="19"/>
       <c r="V30" s="19"/>
     </row>
-    <row r="31" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A31" s="33" t="s">
         <v>19</v>
       </c>
@@ -5266,10 +5268,10 @@
         <v>129</v>
       </c>
       <c r="K31" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L31" s="34" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M31" s="19"/>
       <c r="N31" s="19"/>
@@ -5282,7 +5284,7 @@
       <c r="U31" s="19"/>
       <c r="V31" s="19"/>
     </row>
-    <row r="32" spans="1:22" s="35" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" s="35" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A32" s="36" t="s">
         <v>20</v>
       </c>
@@ -5314,10 +5316,10 @@
         <v>129</v>
       </c>
       <c r="K32" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L32" s="34" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="M32" s="19"/>
       <c r="N32" s="19"/>
@@ -5330,7 +5332,7 @@
       <c r="U32" s="19"/>
       <c r="V32" s="19"/>
     </row>
-    <row r="33" spans="1:22" s="35" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" s="35" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A33" s="36" t="s">
         <v>59</v>
       </c>
@@ -5359,13 +5361,13 @@
         <v>112</v>
       </c>
       <c r="J33" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K33" s="14" t="s">
+        <v>354</v>
+      </c>
+      <c r="L33" s="47" t="s">
         <v>355</v>
-      </c>
-      <c r="L33" s="47" t="s">
-        <v>356</v>
       </c>
       <c r="M33" s="19"/>
       <c r="N33" s="19"/>
@@ -5378,7 +5380,7 @@
       <c r="U33" s="19"/>
       <c r="V33" s="19"/>
     </row>
-    <row r="34" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A34" s="36" t="s">
         <v>21</v>
       </c>
@@ -5410,10 +5412,10 @@
         <v>103</v>
       </c>
       <c r="K34" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L34" s="34" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="M34" s="19"/>
       <c r="N34" s="19"/>
@@ -5426,7 +5428,7 @@
       <c r="U34" s="19"/>
       <c r="V34" s="19"/>
     </row>
-    <row r="35" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A35" s="36" t="s">
         <v>22</v>
       </c>
@@ -5458,10 +5460,10 @@
         <v>103</v>
       </c>
       <c r="K35" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L35" s="34" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M35" s="19"/>
       <c r="N35" s="19"/>
@@ -5474,7 +5476,7 @@
       <c r="U35" s="19"/>
       <c r="V35" s="19"/>
     </row>
-    <row r="36" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A36" s="36" t="s">
         <v>23</v>
       </c>
@@ -5506,10 +5508,10 @@
         <v>103</v>
       </c>
       <c r="K36" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L36" s="34" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M36" s="19"/>
       <c r="N36" s="19"/>
@@ -5522,7 +5524,7 @@
       <c r="U36" s="19"/>
       <c r="V36" s="19"/>
     </row>
-    <row r="37" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A37" s="36" t="s">
         <v>24</v>
       </c>
@@ -5533,10 +5535,10 @@
         <v>25</v>
       </c>
       <c r="D37" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="E37" s="17" t="s">
         <v>300</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>301</v>
       </c>
       <c r="F37" s="17" t="s">
         <v>85</v>
@@ -5554,10 +5556,10 @@
         <v>103</v>
       </c>
       <c r="K37" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="L37" s="34" t="s">
         <v>348</v>
-      </c>
-      <c r="L37" s="34" t="s">
-        <v>349</v>
       </c>
       <c r="M37" s="19"/>
       <c r="N37" s="19"/>
@@ -5570,9 +5572,9 @@
       <c r="U37" s="19"/>
       <c r="V37" s="19"/>
     </row>
-    <row r="38" spans="1:22" s="35" customFormat="1" ht="82.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:22" s="35" customFormat="1" ht="82.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="36" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>140</v>
@@ -5581,10 +5583,10 @@
         <v>43</v>
       </c>
       <c r="D38" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="E38" s="17" t="s">
         <v>362</v>
-      </c>
-      <c r="E38" s="17" t="s">
-        <v>363</v>
       </c>
       <c r="F38" s="17" t="s">
         <v>85</v>
@@ -5599,13 +5601,13 @@
         <v>112</v>
       </c>
       <c r="J38" s="17" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="K38" s="14">
         <v>2017</v>
       </c>
       <c r="L38" s="34" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="M38" s="19"/>
       <c r="N38" s="19"/>
@@ -5618,7 +5620,7 @@
       <c r="U38" s="19"/>
       <c r="V38" s="19"/>
     </row>
-    <row r="39" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A39" s="33" t="s">
         <v>25</v>
       </c>
@@ -5650,10 +5652,10 @@
         <v>97</v>
       </c>
       <c r="K39" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L39" s="34" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="M39" s="19"/>
       <c r="N39" s="19"/>
@@ -5666,7 +5668,7 @@
       <c r="U39" s="19"/>
       <c r="V39" s="19"/>
     </row>
-    <row r="40" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A40" s="33" t="s">
         <v>26</v>
       </c>
@@ -5698,10 +5700,10 @@
         <v>97</v>
       </c>
       <c r="K40" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L40" s="34" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="M40" s="19"/>
       <c r="N40" s="19"/>
@@ -5714,7 +5716,7 @@
       <c r="U40" s="19"/>
       <c r="V40" s="19"/>
     </row>
-    <row r="41" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A41" s="33" t="s">
         <v>27</v>
       </c>
@@ -5746,10 +5748,10 @@
         <v>97</v>
       </c>
       <c r="K41" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L41" s="34" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="M41" s="19"/>
       <c r="N41" s="19"/>
@@ -5762,7 +5764,7 @@
       <c r="U41" s="19"/>
       <c r="V41" s="19"/>
     </row>
-    <row r="42" spans="1:22" s="35" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" s="35" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.15">
       <c r="A42" s="36" t="s">
         <v>232</v>
       </c>
@@ -5794,10 +5796,10 @@
         <v>245</v>
       </c>
       <c r="K42" s="45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L42" s="45" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="M42" s="19"/>
       <c r="N42" s="19"/>
@@ -5810,7 +5812,7 @@
       <c r="U42" s="19"/>
       <c r="V42" s="19"/>
     </row>
-    <row r="43" spans="1:22" s="35" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" s="35" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.15">
       <c r="A43" s="33" t="s">
         <v>28</v>
       </c>
@@ -5842,10 +5844,10 @@
         <v>97</v>
       </c>
       <c r="K43" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L43" s="34" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="M43" s="19"/>
       <c r="N43" s="19"/>
@@ -5858,7 +5860,7 @@
       <c r="U43" s="19"/>
       <c r="V43" s="19"/>
     </row>
-    <row r="44" spans="1:22" s="35" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" s="35" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A44" s="36" t="s">
         <v>233</v>
       </c>
@@ -5887,13 +5889,13 @@
         <v>112</v>
       </c>
       <c r="J44" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K44" s="45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L44" s="47" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="M44" s="19"/>
       <c r="N44" s="19"/>
@@ -5906,7 +5908,7 @@
       <c r="U44" s="19"/>
       <c r="V44" s="19"/>
     </row>
-    <row r="45" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A45" s="36" t="s">
         <v>231</v>
       </c>
@@ -5935,13 +5937,13 @@
         <v>172</v>
       </c>
       <c r="J45" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K45" s="45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L45" s="47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M45" s="19"/>
       <c r="N45" s="19"/>
@@ -5954,7 +5956,7 @@
       <c r="U45" s="19"/>
       <c r="V45" s="19"/>
     </row>
-    <row r="46" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A46" s="36" t="s">
         <v>64</v>
       </c>
@@ -5983,13 +5985,13 @@
         <v>172</v>
       </c>
       <c r="J46" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K46" s="45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L46" s="47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M46" s="19"/>
       <c r="N46" s="19"/>
@@ -6002,7 +6004,7 @@
       <c r="U46" s="19"/>
       <c r="V46" s="19"/>
     </row>
-    <row r="47" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A47" s="36" t="s">
         <v>61</v>
       </c>
@@ -6031,13 +6033,13 @@
         <v>172</v>
       </c>
       <c r="J47" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K47" s="45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L47" s="47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M47" s="19"/>
       <c r="N47" s="19"/>
@@ -6050,7 +6052,7 @@
       <c r="U47" s="19"/>
       <c r="V47" s="19"/>
     </row>
-    <row r="48" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A48" s="36" t="s">
         <v>62</v>
       </c>
@@ -6079,13 +6081,13 @@
         <v>172</v>
       </c>
       <c r="J48" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K48" s="45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L48" s="47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M48" s="19"/>
       <c r="N48" s="19"/>
@@ -6098,7 +6100,7 @@
       <c r="U48" s="19"/>
       <c r="V48" s="19"/>
     </row>
-    <row r="49" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A49" s="36" t="s">
         <v>66</v>
       </c>
@@ -6127,13 +6129,13 @@
         <v>172</v>
       </c>
       <c r="J49" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K49" s="45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L49" s="47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M49" s="19"/>
       <c r="N49" s="19"/>
@@ -6146,7 +6148,7 @@
       <c r="U49" s="19"/>
       <c r="V49" s="19"/>
     </row>
-    <row r="50" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A50" s="36" t="s">
         <v>65</v>
       </c>
@@ -6175,13 +6177,13 @@
         <v>172</v>
       </c>
       <c r="J50" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K50" s="45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L50" s="47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M50" s="19"/>
       <c r="N50" s="19"/>
@@ -6194,7 +6196,7 @@
       <c r="U50" s="19"/>
       <c r="V50" s="19"/>
     </row>
-    <row r="51" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A51" s="36" t="s">
         <v>63</v>
       </c>
@@ -6223,13 +6225,13 @@
         <v>172</v>
       </c>
       <c r="J51" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K51" s="45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L51" s="47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M51" s="19"/>
       <c r="N51" s="19"/>
@@ -6242,7 +6244,7 @@
       <c r="U51" s="19"/>
       <c r="V51" s="19"/>
     </row>
-    <row r="52" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A52" s="36" t="s">
         <v>60</v>
       </c>
@@ -6271,13 +6273,13 @@
         <v>172</v>
       </c>
       <c r="J52" s="22" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="K52" s="45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L52" s="47" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="M52" s="19"/>
       <c r="N52" s="19"/>
@@ -6290,7 +6292,7 @@
       <c r="U52" s="19"/>
       <c r="V52" s="19"/>
     </row>
-    <row r="53" spans="1:22" s="35" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:22" s="35" customFormat="1" ht="133.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="33" t="s">
         <v>29</v>
       </c>
@@ -6322,10 +6324,10 @@
         <v>152</v>
       </c>
       <c r="K53" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L53" s="34" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="M53" s="19"/>
       <c r="N53" s="19"/>
@@ -6338,7 +6340,7 @@
       <c r="U53" s="19"/>
       <c r="V53" s="19"/>
     </row>
-    <row r="54" spans="1:22" s="35" customFormat="1" ht="132.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:22" s="35" customFormat="1" ht="132.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="33" t="s">
         <v>30</v>
       </c>
@@ -6370,10 +6372,10 @@
         <v>152</v>
       </c>
       <c r="K54" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L54" s="34" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="M54" s="19"/>
       <c r="N54" s="19"/>
@@ -6386,7 +6388,7 @@
       <c r="U54" s="19"/>
       <c r="V54" s="19"/>
     </row>
-    <row r="55" spans="1:22" s="35" customFormat="1" ht="165.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:22" s="35" customFormat="1" ht="168" hidden="1" x14ac:dyDescent="0.15">
       <c r="A55" s="33" t="s">
         <v>31</v>
       </c>
@@ -6415,13 +6417,13 @@
         <v>158</v>
       </c>
       <c r="J55" s="11" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="K55" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L55" s="34" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="M55" s="19"/>
       <c r="N55" s="19"/>
@@ -6434,9 +6436,9 @@
       <c r="U55" s="19"/>
       <c r="V55" s="19"/>
     </row>
-    <row r="56" spans="1:22" s="35" customFormat="1" ht="138" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:22" s="35" customFormat="1" ht="140" hidden="1" x14ac:dyDescent="0.15">
       <c r="A56" s="33" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B56" s="9" t="s">
         <v>155</v>
@@ -6445,10 +6447,10 @@
         <v>63</v>
       </c>
       <c r="D56" s="11" t="s">
+        <v>303</v>
+      </c>
+      <c r="E56" s="11" t="s">
         <v>304</v>
-      </c>
-      <c r="E56" s="11" t="s">
-        <v>305</v>
       </c>
       <c r="F56" s="11" t="s">
         <v>82</v>
@@ -6463,13 +6465,13 @@
         <v>104</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K56" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L56" s="34" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="M56" s="19"/>
       <c r="N56" s="19"/>
@@ -6482,7 +6484,7 @@
       <c r="U56" s="19"/>
       <c r="V56" s="19"/>
     </row>
-    <row r="57" spans="1:22" s="35" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:22" s="35" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A57" s="33" t="s">
         <v>32</v>
       </c>
@@ -6514,10 +6516,10 @@
         <v>159</v>
       </c>
       <c r="K57" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="L57" s="34" t="s">
         <v>376</v>
-      </c>
-      <c r="L57" s="34" t="s">
-        <v>377</v>
       </c>
       <c r="M57" s="19"/>
       <c r="N57" s="19"/>
@@ -6530,7 +6532,7 @@
       <c r="U57" s="19"/>
       <c r="V57" s="19"/>
     </row>
-    <row r="58" spans="1:22" s="46" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:22" s="46" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A58" s="33" t="s">
         <v>33</v>
       </c>
@@ -6559,13 +6561,13 @@
         <v>87</v>
       </c>
       <c r="J58" s="34" t="s">
+        <v>539</v>
+      </c>
+      <c r="K58" s="14" t="s">
+        <v>375</v>
+      </c>
+      <c r="L58" s="34" t="s">
         <v>540</v>
-      </c>
-      <c r="K58" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="L58" s="34" t="s">
-        <v>541</v>
       </c>
       <c r="M58" s="19"/>
       <c r="N58" s="19"/>
@@ -6578,7 +6580,7 @@
       <c r="U58" s="19"/>
       <c r="V58" s="19"/>
     </row>
-    <row r="59" spans="1:22" s="46" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:22" s="46" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A59" s="33" t="s">
         <v>34</v>
       </c>
@@ -6610,10 +6612,10 @@
         <v>159</v>
       </c>
       <c r="K59" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L59" s="34" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M59" s="19"/>
       <c r="N59" s="19"/>
@@ -6626,7 +6628,7 @@
       <c r="U59" s="19"/>
       <c r="V59" s="19"/>
     </row>
-    <row r="60" spans="1:22" s="46" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:22" s="46" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A60" s="33" t="s">
         <v>35</v>
       </c>
@@ -6658,10 +6660,10 @@
         <v>159</v>
       </c>
       <c r="K60" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L60" s="34" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="M60" s="19"/>
       <c r="N60" s="19"/>
@@ -6674,7 +6676,7 @@
       <c r="U60" s="19"/>
       <c r="V60" s="19"/>
     </row>
-    <row r="61" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A61" s="36" t="s">
         <v>36</v>
       </c>
@@ -6706,10 +6708,10 @@
         <v>171</v>
       </c>
       <c r="K61" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L61" s="34" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="M61" s="19"/>
       <c r="N61" s="19"/>
@@ -6722,7 +6724,7 @@
       <c r="U61" s="19"/>
       <c r="V61" s="19"/>
     </row>
-    <row r="62" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A62" s="33" t="s">
         <v>37</v>
       </c>
@@ -6754,7 +6756,7 @@
         <v>226</v>
       </c>
       <c r="K62" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L62" s="34" t="s">
         <v>227</v>
@@ -6770,19 +6772,19 @@
       <c r="U62" s="19"/>
       <c r="V62" s="19"/>
     </row>
-    <row r="63" spans="1:22" s="35" customFormat="1" ht="409.6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:22" s="35" customFormat="1" ht="409.6" hidden="1" x14ac:dyDescent="0.15">
       <c r="A63" s="36" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B63" s="9" t="s">
         <v>173</v>
       </c>
       <c r="C63" s="10"/>
       <c r="D63" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F63" s="17" t="s">
         <v>82</v>
@@ -6794,16 +6796,16 @@
         <v>83</v>
       </c>
       <c r="I63" s="66" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J63" s="66" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K63" s="45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L63" s="47" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="M63" s="19"/>
       <c r="N63" s="19"/>
@@ -6816,19 +6818,19 @@
       <c r="U63" s="19"/>
       <c r="V63" s="19"/>
     </row>
-    <row r="64" spans="1:22" s="35" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:22" s="35" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A64" s="36" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B64" s="9" t="s">
         <v>173</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F64" s="17" t="s">
         <v>82</v>
@@ -6840,16 +6842,16 @@
         <v>83</v>
       </c>
       <c r="I64" s="65" t="s">
+        <v>276</v>
+      </c>
+      <c r="J64" s="65" t="s">
         <v>277</v>
       </c>
-      <c r="J64" s="65" t="s">
-        <v>278</v>
-      </c>
       <c r="K64" s="45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L64" s="47" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="M64" s="19"/>
       <c r="N64" s="19"/>
@@ -6862,9 +6864,9 @@
       <c r="U64" s="19"/>
       <c r="V64" s="19"/>
     </row>
-    <row r="65" spans="1:22" s="35" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" s="35" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A65" s="36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B65" s="9" t="s">
         <v>173</v>
@@ -6873,10 +6875,10 @@
         <v>152</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F65" s="17" t="s">
         <v>82</v>
@@ -6888,16 +6890,16 @@
         <v>83</v>
       </c>
       <c r="I65" s="65" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J65" s="65" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K65" s="45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L65" s="47" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="M65" s="19"/>
       <c r="N65" s="19"/>
@@ -6910,9 +6912,9 @@
       <c r="U65" s="19"/>
       <c r="V65" s="19"/>
     </row>
-    <row r="66" spans="1:22" s="35" customFormat="1" ht="409.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" s="35" customFormat="1" ht="409.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="36" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B66" s="9" t="s">
         <v>173</v>
@@ -6921,10 +6923,10 @@
         <v>152</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E66" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="F66" s="17" t="s">
         <v>82</v>
@@ -6936,16 +6938,16 @@
         <v>83</v>
       </c>
       <c r="I66" s="65" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="J66" s="65" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K66" s="45" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L66" s="47" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="M66" s="19"/>
       <c r="N66" s="19"/>
@@ -6958,7 +6960,7 @@
       <c r="U66" s="19"/>
       <c r="V66" s="19"/>
     </row>
-    <row r="67" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A67" s="33" t="s">
         <v>38</v>
       </c>
@@ -6969,10 +6971,10 @@
         <v>73</v>
       </c>
       <c r="D67" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="E67" s="11" t="s">
         <v>400</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>401</v>
       </c>
       <c r="F67" s="11" t="s">
         <v>82</v>
@@ -6987,13 +6989,13 @@
         <v>172</v>
       </c>
       <c r="J67" s="11" t="s">
+        <v>397</v>
+      </c>
+      <c r="K67" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="L67" s="34" t="s">
         <v>398</v>
-      </c>
-      <c r="K67" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="L67" s="34" t="s">
-        <v>399</v>
       </c>
       <c r="M67" s="19"/>
       <c r="N67" s="19"/>
@@ -7006,7 +7008,7 @@
       <c r="U67" s="19"/>
       <c r="V67" s="19"/>
     </row>
-    <row r="68" spans="1:22" s="35" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" s="35" customFormat="1" ht="196" hidden="1" x14ac:dyDescent="0.15">
       <c r="A68" s="33" t="s">
         <v>39</v>
       </c>
@@ -7032,13 +7034,13 @@
         <v>83</v>
       </c>
       <c r="I68" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J68" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K68" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L68" s="34" t="s">
         <v>230</v>
@@ -7054,7 +7056,7 @@
       <c r="U68" s="19"/>
       <c r="V68" s="19"/>
     </row>
-    <row r="69" spans="1:22" s="35" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" s="35" customFormat="1" ht="196" hidden="1" x14ac:dyDescent="0.15">
       <c r="A69" s="36" t="s">
         <v>235</v>
       </c>
@@ -7065,10 +7067,10 @@
         <v>86</v>
       </c>
       <c r="D69" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="E69" s="35" t="s">
         <v>279</v>
-      </c>
-      <c r="E69" s="35" t="s">
-        <v>280</v>
       </c>
       <c r="F69" s="35" t="s">
         <v>82</v>
@@ -7080,16 +7082,16 @@
         <v>83</v>
       </c>
       <c r="I69" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J69" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K69" s="19">
         <v>2015</v>
       </c>
       <c r="L69" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M69" s="19"/>
       <c r="N69" s="19"/>
@@ -7102,7 +7104,7 @@
       <c r="U69" s="19"/>
       <c r="V69" s="19"/>
     </row>
-    <row r="70" spans="1:22" s="35" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" s="35" customFormat="1" ht="196" hidden="1" x14ac:dyDescent="0.15">
       <c r="A70" s="36" t="s">
         <v>236</v>
       </c>
@@ -7113,10 +7115,10 @@
         <v>87</v>
       </c>
       <c r="D70" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="E70" s="35" t="s">
         <v>279</v>
-      </c>
-      <c r="E70" s="35" t="s">
-        <v>280</v>
       </c>
       <c r="F70" s="35" t="s">
         <v>82</v>
@@ -7128,16 +7130,16 @@
         <v>83</v>
       </c>
       <c r="I70" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J70" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K70" s="19">
         <v>2016</v>
       </c>
       <c r="L70" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M70" s="19"/>
       <c r="N70" s="19"/>
@@ -7150,7 +7152,7 @@
       <c r="U70" s="19"/>
       <c r="V70" s="19"/>
     </row>
-    <row r="71" spans="1:22" s="35" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" s="35" customFormat="1" ht="196" hidden="1" x14ac:dyDescent="0.15">
       <c r="A71" s="36" t="s">
         <v>237</v>
       </c>
@@ -7161,10 +7163,10 @@
         <v>88</v>
       </c>
       <c r="D71" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="E71" s="35" t="s">
         <v>279</v>
-      </c>
-      <c r="E71" s="35" t="s">
-        <v>280</v>
       </c>
       <c r="F71" s="35" t="s">
         <v>82</v>
@@ -7176,16 +7178,16 @@
         <v>83</v>
       </c>
       <c r="I71" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J71" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K71" s="19">
         <v>2017</v>
       </c>
       <c r="L71" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M71" s="19"/>
       <c r="N71" s="19"/>
@@ -7198,7 +7200,7 @@
       <c r="U71" s="19"/>
       <c r="V71" s="19"/>
     </row>
-    <row r="72" spans="1:22" s="35" customFormat="1" ht="193.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" s="35" customFormat="1" ht="196" hidden="1" x14ac:dyDescent="0.15">
       <c r="A72" s="36" t="s">
         <v>238</v>
       </c>
@@ -7209,10 +7211,10 @@
         <v>89</v>
       </c>
       <c r="D72" s="35" t="s">
+        <v>278</v>
+      </c>
+      <c r="E72" s="35" t="s">
         <v>279</v>
-      </c>
-      <c r="E72" s="35" t="s">
-        <v>280</v>
       </c>
       <c r="F72" s="35" t="s">
         <v>82</v>
@@ -7224,16 +7226,16 @@
         <v>83</v>
       </c>
       <c r="I72" s="13" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="J72" s="11" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="K72" s="19">
         <v>2018</v>
       </c>
       <c r="L72" s="37" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M72" s="19"/>
       <c r="N72" s="19"/>
@@ -7246,7 +7248,7 @@
       <c r="U72" s="19"/>
       <c r="V72" s="19"/>
     </row>
-    <row r="73" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A73" s="33" t="s">
         <v>40</v>
       </c>
@@ -7278,10 +7280,10 @@
         <v>181</v>
       </c>
       <c r="K73" s="14" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L73" s="34" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="M73" s="19"/>
       <c r="N73" s="19"/>
@@ -7294,7 +7296,7 @@
       <c r="U73" s="19"/>
       <c r="V73" s="19"/>
     </row>
-    <row r="74" spans="1:22" s="35" customFormat="1" ht="124.2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" s="35" customFormat="1" ht="126" hidden="1" x14ac:dyDescent="0.15">
       <c r="A74" s="33" t="s">
         <v>41</v>
       </c>
@@ -7320,16 +7322,16 @@
         <v>83</v>
       </c>
       <c r="I74" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="J74" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="J74" s="11" t="s">
-        <v>307</v>
-      </c>
       <c r="K74" s="14" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="L74" s="34" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M74" s="19"/>
       <c r="N74" s="19"/>
@@ -7342,7 +7344,7 @@
       <c r="U74" s="19"/>
       <c r="V74" s="19"/>
     </row>
-    <row r="75" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A75" s="48" t="s">
         <v>42</v>
       </c>
@@ -7371,16 +7373,16 @@
         <v>96</v>
       </c>
       <c r="J75" s="50" t="s">
+        <v>391</v>
+      </c>
+      <c r="K75" s="52" t="s">
+        <v>307</v>
+      </c>
+      <c r="L75" s="50" t="s">
+        <v>390</v>
+      </c>
+      <c r="M75" s="19" t="s">
         <v>392</v>
-      </c>
-      <c r="K75" s="52" t="s">
-        <v>308</v>
-      </c>
-      <c r="L75" s="50" t="s">
-        <v>391</v>
-      </c>
-      <c r="M75" s="19" t="s">
-        <v>393</v>
       </c>
       <c r="N75" s="19"/>
       <c r="O75" s="19"/>
@@ -7392,7 +7394,7 @@
       <c r="U75" s="19"/>
       <c r="V75" s="19"/>
     </row>
-    <row r="76" spans="1:22" s="35" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" s="35" customFormat="1" ht="133.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A76" s="36" t="s">
         <v>43</v>
       </c>
@@ -7418,16 +7420,16 @@
         <v>83</v>
       </c>
       <c r="I76" s="18" t="s">
+        <v>394</v>
+      </c>
+      <c r="J76" s="17" t="s">
         <v>395</v>
       </c>
-      <c r="J76" s="17" t="s">
-        <v>396</v>
-      </c>
       <c r="K76" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L76" s="34" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="M76" s="19"/>
       <c r="N76" s="19"/>
@@ -7440,7 +7442,7 @@
       <c r="U76" s="19"/>
       <c r="V76" s="19"/>
     </row>
-    <row r="77" spans="1:22" s="35" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:22" s="35" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.15">
       <c r="A77" s="33" t="s">
         <v>44</v>
       </c>
@@ -7454,7 +7456,7 @@
         <v>188</v>
       </c>
       <c r="E77" s="11" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="F77" s="11" t="s">
         <v>82</v>
@@ -7469,13 +7471,13 @@
         <v>87</v>
       </c>
       <c r="J77" s="11" t="s">
+        <v>290</v>
+      </c>
+      <c r="K77" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="L77" s="34" t="s">
         <v>291</v>
-      </c>
-      <c r="K77" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="L77" s="34" t="s">
-        <v>292</v>
       </c>
       <c r="M77" s="19"/>
       <c r="N77" s="19"/>
@@ -7488,7 +7490,7 @@
       <c r="U77" s="19"/>
       <c r="V77" s="19"/>
     </row>
-    <row r="78" spans="1:22" s="35" customFormat="1" ht="110.4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:22" s="35" customFormat="1" ht="112" hidden="1" x14ac:dyDescent="0.15">
       <c r="A78" s="33" t="s">
         <v>45</v>
       </c>
@@ -7517,13 +7519,13 @@
         <v>172</v>
       </c>
       <c r="J78" s="11" t="s">
+        <v>287</v>
+      </c>
+      <c r="K78" s="14" t="s">
+        <v>307</v>
+      </c>
+      <c r="L78" s="34" t="s">
         <v>288</v>
-      </c>
-      <c r="K78" s="14" t="s">
-        <v>308</v>
-      </c>
-      <c r="L78" s="34" t="s">
-        <v>289</v>
       </c>
       <c r="M78" s="19"/>
       <c r="N78" s="19"/>
@@ -7536,7 +7538,7 @@
       <c r="U78" s="19"/>
       <c r="V78" s="19"/>
     </row>
-    <row r="79" spans="1:22" s="35" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:22" s="35" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.15">
       <c r="A79" s="33" t="s">
         <v>46</v>
       </c>
@@ -7563,13 +7565,13 @@
       </c>
       <c r="I79" s="13"/>
       <c r="J79" s="11" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="K79" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L79" s="34" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="M79" s="19"/>
       <c r="N79" s="19"/>
@@ -7582,7 +7584,7 @@
       <c r="U79" s="19"/>
       <c r="V79" s="19"/>
     </row>
-    <row r="80" spans="1:22" s="35" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:22" s="35" customFormat="1" ht="28" hidden="1" x14ac:dyDescent="0.15">
       <c r="A80" s="33" t="s">
         <v>47</v>
       </c>
@@ -7609,10 +7611,10 @@
       </c>
       <c r="I80" s="13"/>
       <c r="J80" s="11" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K80" s="14" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="L80" s="34"/>
       <c r="M80" s="19"/>
@@ -7626,7 +7628,7 @@
       <c r="U80" s="19"/>
       <c r="V80" s="19"/>
     </row>
-    <row r="81" spans="1:22" s="35" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:22" s="35" customFormat="1" ht="56" x14ac:dyDescent="0.15">
       <c r="A81" s="38" t="s">
         <v>48</v>
       </c>
@@ -7670,7 +7672,7 @@
       <c r="U81" s="19"/>
       <c r="V81" s="19"/>
     </row>
-    <row r="82" spans="1:22" s="35" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:22" s="35" customFormat="1" ht="70" hidden="1" x14ac:dyDescent="0.15">
       <c r="A82" s="33" t="s">
         <v>49</v>
       </c>
@@ -7702,7 +7704,7 @@
         <v>201</v>
       </c>
       <c r="K82" s="14" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="L82" s="34"/>
       <c r="M82" s="19"/>
@@ -7716,7 +7718,7 @@
       <c r="U82" s="19"/>
       <c r="V82" s="19"/>
     </row>
-    <row r="83" spans="1:22" s="35" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:22" s="35" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A83" s="36" t="s">
         <v>234</v>
       </c>
@@ -7748,7 +7750,7 @@
         <v>268</v>
       </c>
       <c r="K83" s="58" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L83" s="19"/>
       <c r="M83" s="19"/>
@@ -7762,9 +7764,9 @@
       <c r="U83" s="19"/>
       <c r="V83" s="19"/>
     </row>
-    <row r="84" spans="1:22" s="35" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:22" s="35" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A84" s="36" t="s">
-        <v>271</v>
+        <v>542</v>
       </c>
       <c r="B84" s="9" t="s">
         <v>173</v>
@@ -7773,10 +7775,10 @@
         <v>83</v>
       </c>
       <c r="D84" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="E84" s="17" t="s">
         <v>272</v>
-      </c>
-      <c r="E84" s="17" t="s">
-        <v>273</v>
       </c>
       <c r="F84" s="17" t="s">
         <v>82</v>
@@ -7794,7 +7796,7 @@
         <v>268</v>
       </c>
       <c r="K84" s="58" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L84" s="19"/>
       <c r="M84" s="19"/>
@@ -7808,7 +7810,7 @@
       <c r="U84" s="19"/>
       <c r="V84" s="19"/>
     </row>
-    <row r="85" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A85" s="33" t="s">
         <v>50</v>
       </c>
@@ -7840,10 +7842,10 @@
         <v>97</v>
       </c>
       <c r="K85" s="44" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L85" s="34" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="M85" s="19"/>
       <c r="N85" s="19"/>
@@ -7856,7 +7858,7 @@
       <c r="U85" s="19"/>
       <c r="V85" s="19"/>
     </row>
-    <row r="86" spans="1:22" s="35" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:22" s="35" customFormat="1" ht="56" hidden="1" x14ac:dyDescent="0.15">
       <c r="A86" s="36" t="s">
         <v>67</v>
       </c>
@@ -7867,10 +7869,10 @@
         <v>52</v>
       </c>
       <c r="D86" s="16" t="s">
+        <v>273</v>
+      </c>
+      <c r="E86" s="17" t="s">
         <v>274</v>
-      </c>
-      <c r="E86" s="17" t="s">
-        <v>275</v>
       </c>
       <c r="F86" s="17" t="s">
         <v>82</v>
@@ -7888,7 +7890,7 @@
         <v>245</v>
       </c>
       <c r="K86" s="45" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L86" s="19"/>
       <c r="M86" s="19"/>
@@ -7902,7 +7904,7 @@
       <c r="U86" s="19"/>
       <c r="V86" s="19"/>
     </row>
-    <row r="87" spans="1:22" s="46" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:22" s="46" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A87" s="54" t="s">
         <v>51</v>
       </c>
@@ -7934,13 +7936,13 @@
         <v>129</v>
       </c>
       <c r="K87" s="52" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L87" s="50" t="s">
         <v>228</v>
       </c>
       <c r="M87" s="19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N87" s="19"/>
       <c r="O87" s="19"/>
@@ -7952,7 +7954,7 @@
       <c r="U87" s="19"/>
       <c r="V87" s="19"/>
     </row>
-    <row r="88" spans="1:22" s="46" customFormat="1" ht="82.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:22" s="46" customFormat="1" ht="84" hidden="1" x14ac:dyDescent="0.15">
       <c r="A88" s="54" t="s">
         <v>52</v>
       </c>
@@ -7984,13 +7986,13 @@
         <v>129</v>
       </c>
       <c r="K88" s="52" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="L88" s="50" t="s">
         <v>228</v>
       </c>
       <c r="M88" s="19" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="N88" s="19"/>
       <c r="O88" s="19"/>
@@ -8002,7 +8004,7 @@
       <c r="U88" s="19"/>
       <c r="V88" s="19"/>
     </row>
-    <row r="89" spans="1:22" s="35" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:22" s="35" customFormat="1" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A89" s="36" t="s">
         <v>53</v>
       </c>
@@ -8031,13 +8033,13 @@
         <v>96</v>
       </c>
       <c r="J89" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K89" s="14" t="s">
         <v>225</v>
       </c>
       <c r="L89" s="34" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M89" s="19"/>
       <c r="N89" s="19"/>
@@ -8050,7 +8052,7 @@
       <c r="U89" s="19"/>
       <c r="V89" s="19"/>
     </row>
-    <row r="90" spans="1:22" s="35" customFormat="1" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:22" s="35" customFormat="1" ht="98" hidden="1" x14ac:dyDescent="0.15">
       <c r="A90" s="36" t="s">
         <v>54</v>
       </c>
@@ -8096,7 +8098,7 @@
       <c r="U90" s="19"/>
       <c r="V90" s="19"/>
     </row>
-    <row r="91" spans="1:22" s="35" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:22" s="35" customFormat="1" ht="89.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A91" s="36" t="s">
         <v>55</v>
       </c>
@@ -8142,7 +8144,7 @@
       <c r="U91" s="19"/>
       <c r="V91" s="19"/>
     </row>
-    <row r="92" spans="1:22" s="35" customFormat="1" ht="89.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:22" s="35" customFormat="1" ht="89.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A92" s="36" t="s">
         <v>56</v>
       </c>
@@ -8188,9 +8190,9 @@
       <c r="U92" s="19"/>
       <c r="V92" s="19"/>
     </row>
-    <row r="93" spans="1:22" s="35" customFormat="1" ht="79.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:22" s="35" customFormat="1" ht="79.5" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A93" s="36" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B93" s="9" t="s">
         <v>202</v>
@@ -8199,10 +8201,10 @@
         <v>59</v>
       </c>
       <c r="D93" s="16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="F93" s="17" t="s">
         <v>85</v>
@@ -8217,7 +8219,7 @@
         <v>112</v>
       </c>
       <c r="J93" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K93" s="14">
         <v>2017</v>
@@ -8234,9 +8236,9 @@
       <c r="U93" s="19"/>
       <c r="V93" s="19"/>
     </row>
-    <row r="94" spans="1:22" s="35" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:22" s="35" customFormat="1" ht="83.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A94" s="36" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B94" s="9" t="s">
         <v>202</v>
@@ -8245,10 +8247,10 @@
         <v>60</v>
       </c>
       <c r="D94" s="16" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E94" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="F94" s="17" t="s">
         <v>85</v>
@@ -8263,7 +8265,7 @@
         <v>112</v>
       </c>
       <c r="J94" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="K94" s="14">
         <v>2017</v>
@@ -8280,9 +8282,9 @@
       <c r="U94" s="19"/>
       <c r="V94" s="19"/>
     </row>
-    <row r="95" spans="1:22" s="35" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:22" s="35" customFormat="1" ht="83.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A95" s="36" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B95" s="9" t="s">
         <v>202</v>
@@ -8291,10 +8293,10 @@
         <v>90</v>
       </c>
       <c r="D95" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="E95" s="17" t="s">
         <v>389</v>
-      </c>
-      <c r="E95" s="17" t="s">
-        <v>390</v>
       </c>
       <c r="F95" s="17" t="s">
         <v>85</v>
@@ -8307,7 +8309,7 @@
       </c>
       <c r="I95" s="18"/>
       <c r="J95" s="17" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K95" s="14">
         <v>2017</v>
@@ -8324,9 +8326,9 @@
       <c r="U95" s="19"/>
       <c r="V95" s="19"/>
     </row>
-    <row r="96" spans="1:22" s="35" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:22" s="35" customFormat="1" ht="83.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="36" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B96" s="9" t="s">
         <v>202</v>
@@ -8335,10 +8337,10 @@
         <v>91</v>
       </c>
       <c r="D96" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="E96" s="17" t="s">
         <v>389</v>
-      </c>
-      <c r="E96" s="17" t="s">
-        <v>390</v>
       </c>
       <c r="F96" s="17" t="s">
         <v>85</v>
@@ -8351,7 +8353,7 @@
       </c>
       <c r="I96" s="18"/>
       <c r="J96" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K96" s="14">
         <v>2017</v>
@@ -8368,9 +8370,9 @@
       <c r="U96" s="19"/>
       <c r="V96" s="19"/>
     </row>
-    <row r="97" spans="1:22" s="35" customFormat="1" ht="83.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:22" s="35" customFormat="1" ht="83.25" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A97" s="36" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B97" s="9" t="s">
         <v>202</v>
@@ -8379,10 +8381,10 @@
         <v>92</v>
       </c>
       <c r="D97" s="16" t="s">
+        <v>388</v>
+      </c>
+      <c r="E97" s="17" t="s">
         <v>389</v>
-      </c>
-      <c r="E97" s="17" t="s">
-        <v>390</v>
       </c>
       <c r="F97" s="17" t="s">
         <v>85</v>
@@ -8395,7 +8397,7 @@
       </c>
       <c r="I97" s="18"/>
       <c r="J97" s="17" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="K97" s="14">
         <v>2017</v>
@@ -8412,7 +8414,7 @@
       <c r="U97" s="19"/>
       <c r="V97" s="19"/>
     </row>
-    <row r="98" spans="1:22" s="35" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:22" s="35" customFormat="1" ht="42" hidden="1" x14ac:dyDescent="0.15">
       <c r="A98" s="36" t="s">
         <v>57</v>
       </c>
@@ -8443,7 +8445,7 @@
         <v>229</v>
       </c>
       <c r="L98" s="34" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="M98" s="19"/>
       <c r="N98" s="19"/>
@@ -8456,11 +8458,17 @@
       <c r="U98" s="19"/>
       <c r="V98" s="19"/>
     </row>
-    <row r="99" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A99" s="39"/>
     </row>
   </sheetData>
-  <autoFilter ref="A4:L98"/>
+  <autoFilter ref="A4:L98" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="region"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="3">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -8473,714 +8481,714 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" style="71" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.109375" style="71"/>
+    <col min="1" max="1" width="12.5" style="71" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.1640625" style="71"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A1" s="69" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B1" s="70"/>
       <c r="C1" s="70"/>
     </row>
-    <row r="2" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A2" s="69">
         <v>1</v>
       </c>
       <c r="B2" s="68" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C2" s="70"/>
     </row>
-    <row r="3" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" s="69">
         <v>2</v>
       </c>
       <c r="B3" s="68" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C3" s="70"/>
     </row>
-    <row r="4" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" s="69">
         <v>3</v>
       </c>
       <c r="B4" s="68" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C4" s="70"/>
     </row>
-    <row r="5" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A5" s="69">
         <v>4</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C5" s="70"/>
     </row>
-    <row r="6" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="69"/>
       <c r="B6" s="70"/>
       <c r="C6" s="70"/>
     </row>
-    <row r="7" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" s="69" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B7" s="70"/>
       <c r="C7" s="70"/>
     </row>
-    <row r="8" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" s="69">
         <v>100</v>
       </c>
       <c r="B8" s="68" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C8" s="70"/>
     </row>
-    <row r="9" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" s="69">
         <v>101</v>
       </c>
       <c r="B9" s="68" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C9" s="70"/>
     </row>
-    <row r="10" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" s="69">
         <v>102</v>
       </c>
       <c r="B10" s="68" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C10" s="70"/>
     </row>
-    <row r="11" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" s="69">
         <v>103</v>
       </c>
       <c r="B11" s="68" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C11" s="70"/>
     </row>
-    <row r="12" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A12" s="69">
         <v>104</v>
       </c>
       <c r="B12" s="68" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C12" s="70"/>
     </row>
-    <row r="13" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" s="69">
         <v>105</v>
       </c>
       <c r="B13" s="68" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C13" s="70"/>
     </row>
-    <row r="14" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" s="69">
         <v>106</v>
       </c>
       <c r="B14" s="68" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C14" s="70"/>
     </row>
-    <row r="15" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" s="69"/>
       <c r="B15" s="70"/>
       <c r="C15" s="70"/>
     </row>
-    <row r="16" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="69" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B16" s="70"/>
       <c r="C16" s="70"/>
     </row>
-    <row r="17" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" s="69">
         <v>200</v>
       </c>
       <c r="B17" s="68" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C17" s="70"/>
     </row>
-    <row r="18" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" s="69">
         <v>201</v>
       </c>
       <c r="B18" s="68" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C18" s="70"/>
     </row>
-    <row r="19" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" s="69">
         <v>202</v>
       </c>
       <c r="B19" s="68" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C19" s="70"/>
     </row>
-    <row r="20" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" s="69"/>
       <c r="B20" s="70"/>
       <c r="C20" s="70"/>
     </row>
-    <row r="21" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" s="69" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B21" s="70"/>
       <c r="C21" s="70"/>
     </row>
-    <row r="22" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" s="69">
         <v>6</v>
       </c>
       <c r="B22" s="68" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C22" s="70"/>
     </row>
-    <row r="23" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" s="69">
         <v>300</v>
       </c>
       <c r="B23" s="68" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C23" s="70"/>
     </row>
-    <row r="24" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A24" s="69">
         <v>301</v>
       </c>
       <c r="B24" s="68" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C24" s="70"/>
     </row>
-    <row r="25" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="69">
         <v>302</v>
       </c>
       <c r="B25" s="68" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C25" s="70"/>
     </row>
-    <row r="26" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" s="69">
         <v>303</v>
       </c>
       <c r="B26" s="68" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C26" s="70"/>
     </row>
-    <row r="27" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" s="69">
         <v>304</v>
       </c>
       <c r="B27" s="68" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C27" s="70"/>
     </row>
-    <row r="28" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="69">
         <v>305</v>
       </c>
       <c r="B28" s="68" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C28" s="70"/>
     </row>
-    <row r="29" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="69">
         <v>306</v>
       </c>
       <c r="B29" s="68" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C29" s="70"/>
     </row>
-    <row r="30" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" s="69"/>
       <c r="B30" s="70"/>
       <c r="C30" s="70"/>
     </row>
-    <row r="31" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" s="69" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B31" s="70"/>
       <c r="C31" s="70"/>
     </row>
-    <row r="32" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" s="69">
         <v>400</v>
       </c>
       <c r="B32" s="68" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="C32" s="70"/>
     </row>
-    <row r="33" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" s="69">
         <v>401</v>
       </c>
       <c r="B33" s="68" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C33" s="70"/>
     </row>
-    <row r="34" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" s="69">
         <v>402</v>
       </c>
       <c r="B34" s="68" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C34" s="70"/>
     </row>
-    <row r="35" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" s="69">
         <v>403</v>
       </c>
       <c r="B35" s="68" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="C35" s="70"/>
     </row>
-    <row r="36" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A36" s="69"/>
       <c r="B36" s="70"/>
       <c r="C36" s="70"/>
     </row>
-    <row r="37" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A37" s="69" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B37" s="70"/>
       <c r="C37" s="70"/>
     </row>
-    <row r="38" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A38" s="69">
         <v>500</v>
       </c>
       <c r="B38" s="68" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="C38" s="70"/>
     </row>
-    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A39" s="69">
         <v>501</v>
       </c>
       <c r="B39" s="68" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C39" s="70"/>
     </row>
-    <row r="40" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A40" s="69">
         <v>502</v>
       </c>
       <c r="B40" s="68" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C40" s="70"/>
     </row>
-    <row r="41" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A41" s="69">
         <v>503</v>
       </c>
       <c r="B41" s="68" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C41" s="70"/>
     </row>
-    <row r="42" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A42" s="69">
         <v>504</v>
       </c>
       <c r="B42" s="68" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C42" s="70"/>
     </row>
-    <row r="43" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A43" s="69">
         <v>600</v>
       </c>
       <c r="B43" s="68" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C43" s="70"/>
     </row>
-    <row r="44" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A44" s="69">
         <v>601</v>
       </c>
       <c r="B44" s="68" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C44" s="70"/>
     </row>
-    <row r="45" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A45" s="69">
         <v>602</v>
       </c>
       <c r="B45" s="68" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C45" s="70"/>
     </row>
-    <row r="46" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A46" s="69"/>
       <c r="B46" s="70"/>
       <c r="C46" s="70"/>
     </row>
-    <row r="47" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A47" s="69" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B47" s="70"/>
       <c r="C47" s="70"/>
     </row>
-    <row r="48" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A48" s="69">
         <v>700</v>
       </c>
       <c r="B48" s="68" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C48" s="70"/>
     </row>
-    <row r="49" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A49" s="69">
         <v>701</v>
       </c>
       <c r="B49" s="68" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C49" s="70"/>
     </row>
-    <row r="50" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A50" s="69">
         <v>702</v>
       </c>
       <c r="B50" s="68" t="s">
+        <v>505</v>
+      </c>
+      <c r="C50" s="70"/>
+    </row>
+    <row r="51" spans="1:3" ht="16" x14ac:dyDescent="0.15">
+      <c r="A51" s="69" t="s">
         <v>506</v>
       </c>
-      <c r="C50" s="70"/>
-    </row>
-    <row r="51" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
-      <c r="A51" s="69" t="s">
+      <c r="B51" s="68" t="s">
         <v>507</v>
       </c>
-      <c r="B51" s="68" t="s">
-        <v>508</v>
-      </c>
       <c r="C51" s="70"/>
     </row>
-    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A52" s="69">
         <v>704</v>
       </c>
       <c r="B52" s="68" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C52" s="70"/>
     </row>
-    <row r="53" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A53" s="69">
         <v>705</v>
       </c>
       <c r="B53" s="68" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="C53" s="70"/>
     </row>
-    <row r="54" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A54" s="69">
         <v>706</v>
       </c>
       <c r="B54" s="68" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C54" s="70"/>
     </row>
-    <row r="55" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A55" s="69">
         <v>707</v>
       </c>
       <c r="B55" s="68" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C55" s="70"/>
     </row>
-    <row r="56" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A56" s="69">
         <v>708</v>
       </c>
       <c r="B56" s="68" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C56" s="70"/>
     </row>
-    <row r="57" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A57" s="69"/>
       <c r="B57" s="70"/>
       <c r="C57" s="70"/>
     </row>
-    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A58" s="69" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B58" s="70"/>
       <c r="C58" s="70"/>
     </row>
-    <row r="59" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A59" s="69">
         <v>800</v>
       </c>
       <c r="B59" s="68" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C59" s="70"/>
     </row>
-    <row r="60" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A60" s="69">
         <v>801</v>
       </c>
       <c r="B60" s="68" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C60" s="70"/>
     </row>
-    <row r="61" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A61" s="69">
         <v>802</v>
       </c>
       <c r="B61" s="68" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C61" s="70"/>
     </row>
-    <row r="62" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A62" s="69">
         <v>803</v>
       </c>
       <c r="B62" s="68" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C62" s="70"/>
     </row>
-    <row r="63" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A63" s="69">
         <v>804</v>
       </c>
       <c r="B63" s="68" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C63" s="70"/>
     </row>
-    <row r="64" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A64" s="69">
         <v>805</v>
       </c>
       <c r="B64" s="68" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C64" s="70"/>
     </row>
-    <row r="65" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A65" s="69">
         <v>806</v>
       </c>
       <c r="B65" s="68" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C65" s="70"/>
     </row>
-    <row r="66" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A66" s="69">
         <v>807</v>
       </c>
       <c r="B66" s="68" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C66" s="70"/>
     </row>
-    <row r="67" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A67" s="69"/>
       <c r="B67" s="70"/>
       <c r="C67" s="70"/>
     </row>
-    <row r="68" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A68" s="69" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B68" s="70"/>
       <c r="C68" s="70"/>
     </row>
-    <row r="69" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A69" s="69">
         <v>5</v>
       </c>
       <c r="B69" s="68" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C69" s="70"/>
     </row>
-    <row r="70" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A70" s="69">
         <v>900</v>
       </c>
       <c r="B70" s="68" t="s">
+        <v>524</v>
+      </c>
+      <c r="C70" s="68" t="s">
         <v>525</v>
       </c>
-      <c r="C70" s="68" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A71" s="69">
         <v>901</v>
       </c>
       <c r="B71" s="68" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C71" s="70"/>
     </row>
-    <row r="72" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A72" s="69">
         <v>902</v>
       </c>
       <c r="B72" s="68" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C72" s="70"/>
     </row>
-    <row r="73" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A73" s="69">
         <v>903</v>
       </c>
       <c r="B73" s="68" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C73" s="70"/>
     </row>
-    <row r="74" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A74" s="69">
         <v>904</v>
       </c>
       <c r="B74" s="68" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C74" s="70"/>
     </row>
-    <row r="75" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A75" s="69">
         <v>905</v>
       </c>
       <c r="B75" s="68" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C75" s="70"/>
     </row>
-    <row r="76" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A76" s="69"/>
       <c r="B76" s="70"/>
       <c r="C76" s="70"/>
     </row>
-    <row r="77" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A77" s="69" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B77" s="70"/>
       <c r="C77" s="70"/>
     </row>
-    <row r="78" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A78" s="69">
         <v>1000</v>
       </c>
       <c r="B78" s="68" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C78" s="70"/>
     </row>
-    <row r="79" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A79" s="69">
         <v>1001</v>
       </c>
       <c r="B79" s="68" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C79" s="70"/>
     </row>
-    <row r="80" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A80" s="69">
         <v>1002</v>
       </c>
       <c r="B80" s="68" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C80" s="70"/>
     </row>
-    <row r="81" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A81" s="69">
         <v>1003</v>
       </c>
       <c r="B81" s="68" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C81" s="70"/>
     </row>
-    <row r="82" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A82" s="69"/>
       <c r="B82" s="70"/>
       <c r="C82" s="70"/>
     </row>
-    <row r="83" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A83" s="69">
         <v>9999</v>
       </c>
       <c r="B83" s="68" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="C83" s="70"/>
     </row>
-    <row r="84" spans="1:3" ht="15.6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="16" x14ac:dyDescent="0.15">
       <c r="A84" s="69">
         <v>0</v>
       </c>
       <c r="B84" s="68" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C84" s="70"/>
     </row>
@@ -9191,390 +9199,390 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:C49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.15">
       <c r="B2" s="67" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" ht="13.8" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="4" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="59">
         <v>1</v>
       </c>
       <c r="C4" s="62" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="60">
         <v>2</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="60">
         <v>3</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="60">
         <v>4</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="60">
         <v>5</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="9" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="60">
         <v>6</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="10" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="60">
         <v>7</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="11" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="60">
         <v>8</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="60">
         <v>9</v>
       </c>
       <c r="C12" s="63" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B13" s="60">
+        <v>10</v>
+      </c>
+      <c r="C13" s="63" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="13" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="60">
-        <v>10</v>
-      </c>
-      <c r="C13" s="63" t="s">
-        <v>417</v>
-      </c>
-    </row>
-    <row r="14" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B14" s="60">
         <v>11</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="15" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="60">
         <v>12</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="60">
         <v>13</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="60">
         <v>14</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B18" s="60">
         <v>15</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="60">
         <v>16</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="60">
         <v>17</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="60">
         <v>18</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="22" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B22" s="60">
         <v>19</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="23" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B23" s="60">
         <v>20</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B24" s="60">
         <v>21</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B25" s="60">
         <v>22</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="60">
         <v>23</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B27" s="60">
         <v>24</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>431</v>
-      </c>
-    </row>
-    <row r="28" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B28" s="60">
         <v>25</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B29" s="60">
         <v>26</v>
       </c>
       <c r="C29" s="63" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="60">
         <v>27</v>
       </c>
       <c r="C30" s="63" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B31" s="60">
         <v>28</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B32" s="60">
         <v>29</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B33" s="60">
         <v>30</v>
       </c>
       <c r="C33" s="63" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B34" s="60">
         <v>31</v>
       </c>
       <c r="C34" s="63" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B35" s="60">
         <v>32</v>
       </c>
       <c r="C35" s="63" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B36" s="60">
         <v>33</v>
       </c>
       <c r="C36" s="63" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B37" s="60">
         <v>34</v>
       </c>
       <c r="C37" s="63" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B38" s="60">
         <v>35</v>
       </c>
       <c r="C38" s="63" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B39" s="60">
         <v>36</v>
       </c>
       <c r="C39" s="63" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B40" s="60">
         <v>37</v>
       </c>
       <c r="C40" s="63" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B41" s="60">
         <v>38</v>
       </c>
       <c r="C41" s="63" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="60">
         <v>39</v>
       </c>
       <c r="C42" s="63" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B43" s="60">
         <v>40</v>
       </c>
       <c r="C43" s="63" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B44" s="60">
         <v>41</v>
       </c>
       <c r="C44" s="63" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B45" s="60">
         <v>42</v>
       </c>
       <c r="C45" s="63" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B46" s="60">
         <v>43</v>
       </c>
       <c r="C46" s="63" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B47" s="60">
         <v>44</v>
       </c>
       <c r="C47" s="63" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B48" s="60">
         <v>45</v>
       </c>
       <c r="C48" s="63" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B49" s="61">
         <v>46</v>
       </c>
       <c r="C49" s="64" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>

</xml_diff>